<commit_message>
se agrandaron las celdas para ver mejor la información
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuent\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuent\Desktop\Horario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -448,10 +448,17 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
en lunes 13, adelanté prácticas de informática en vez de estudiar calculo integral y el martes también adelanté las prácticas antes de la clase de física
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="36">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>semana del 6 hasta el 10 de marzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adelantar practicas de laboratorio informatica </t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -187,11 +190,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -199,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
@@ -615,7 +630,7 @@
       <c r="A8" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -637,10 +652,12 @@
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6" t="s">
@@ -653,8 +670,12 @@
       <c r="A10" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -665,8 +686,10 @@
       <c r="A11" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -687,7 +710,7 @@
       <c r="A12" s="2">
         <v>0.625</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -719,7 +742,7 @@
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -738,7 +761,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>19</v>
@@ -760,7 +783,7 @@
         <v>0.75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -783,7 +806,9 @@
       <c r="A16" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
@@ -803,7 +828,9 @@
       <c r="A17" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -819,7 +846,7 @@
       <c r="A18" s="2">
         <v>0.875</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="4"/>
@@ -833,11 +860,11 @@
       <c r="A19" s="2">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1" t="s">
@@ -853,7 +880,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="1" t="s">

</xml_diff>

<commit_message>
el miercoles, luego de la clase de vivamos la universidad, estudié cálculo integral y seguí adelantando la práctica de laboratorio de info
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="38">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t xml:space="preserve">adelantar practicas de laboratorio informatica </t>
+  </si>
+  <si>
+    <t>adelantar practicas laboratorio</t>
+  </si>
+  <si>
+    <t>clase-taller física mecánica</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +667,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -678,7 +684,9 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -696,7 +704,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>27</v>
@@ -720,7 +728,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>27</v>
@@ -813,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>20</v>
@@ -833,7 +841,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6" t="s">
@@ -850,7 +858,9 @@
         <v>13</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -867,7 +877,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="4"/>
@@ -883,7 +893,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="4"/>

</xml_diff>

<commit_message>
Acrualición de cambios del sábado, domingo y lunes de algunas horas de estudio, se vieron trocadas por otras y por la práctica de laboratorio de info
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="40">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>clase-taller física mecánica</t>
+  </si>
+  <si>
+    <t>Adelantar prácticas laboratorio informatica</t>
+  </si>
+  <si>
+    <t>Estudiar algebra líneal</t>
   </si>
 </sst>
 </file>
@@ -502,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,9 +740,9 @@
         <v>27</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -760,9 +766,11 @@
         <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -780,11 +788,15 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="G14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1053,7 +1065,7 @@
       <c r="A31" s="2">
         <v>0.5</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="4"/>
@@ -1069,7 +1081,9 @@
       <c r="A32" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1083,7 +1097,7 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -1103,11 +1117,11 @@
       <c r="A34" s="2">
         <v>0.625</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>12</v>
+      <c r="B34" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
@@ -1130,7 +1144,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
@@ -1155,8 +1169,8 @@
       <c r="A36" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>12</v>
+      <c r="B36" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>19</v>
@@ -1177,8 +1191,8 @@
       <c r="A37" s="2">
         <v>0.75</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>12</v>
+      <c r="B37" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>20</v>
@@ -1201,7 +1215,9 @@
       <c r="A38" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1237,8 +1253,8 @@
       <c r="A40" s="2">
         <v>0.875</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>13</v>
+      <c r="B40" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -1252,7 +1268,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>9</v>
@@ -1269,7 +1285,9 @@
       <c r="A42" s="2">
         <v>0.95833333333333337</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Actualización de cambios de la semana pasada desde el 22 hasta hoy 28, algunas horas de estudio se vieron trocadas por la práctica de laboratorio de info y otras razones
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="41">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -144,16 +144,25 @@
   </si>
   <si>
     <t>Estudiar algebra líneal</t>
+  </si>
+  <si>
+    <t>estudiar álgebra lineal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -226,6 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1081,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="4"/>
@@ -1103,9 +1113,9 @@
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1127,13 +1137,13 @@
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>31</v>
@@ -1159,9 +1169,9 @@
         <v>27</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1182,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="4"/>
@@ -1206,8 +1216,8 @@
       <c r="F37" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>31</v>
+      <c r="G37" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="H37" s="4"/>
     </row>
@@ -1239,8 +1249,8 @@
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
-        <v>12</v>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="6" t="s">
@@ -1257,8 +1267,12 @@
         <v>39</v>
       </c>
       <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -1273,9 +1287,11 @@
       <c r="C41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="4"/>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E41" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1291,8 +1307,10 @@
       <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="1" t="s">
+      <c r="D42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F42" s="4"/>
@@ -1430,8 +1448,8 @@
       <c r="A52" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>9</v>
+      <c r="B52" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>16</v>
@@ -1452,8 +1470,8 @@
       <c r="A53" s="2">
         <v>0.5</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>9</v>
+      <c r="B53" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -1468,7 +1486,9 @@
       <c r="A54" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B54" s="4"/>
+      <c r="B54" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1481,7 +1501,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1503,9 +1523,9 @@
         <v>0.625</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1529,7 +1549,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>19</v>
@@ -1637,7 +1657,7 @@
         <v>0.875</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -1651,7 +1671,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>9</v>
@@ -2017,5 +2037,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualización del horario, no estudié más el 28 por la noche, el 1 adelánte prácticas de informática y ayer 2 solo estudié para física mecánica y cálculo integral ya que tenía un parcial ayer 2 y otro parcial hoy 3
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="43">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>estudiar álgebra lineal</t>
+  </si>
+  <si>
+    <t>parcial física mecánica</t>
+  </si>
+  <si>
+    <t>parcial cálculo integral</t>
   </si>
 </sst>
 </file>
@@ -518,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,11 +1401,11 @@
       <c r="D49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>21</v>
+      <c r="F49" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -1415,10 +1421,10 @@
       <c r="D50" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G50" s="4"/>
@@ -1436,10 +1442,10 @@
         <v>22</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -1458,10 +1464,10 @@
         <v>22</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -1476,7 +1482,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G53" s="4"/>
@@ -1504,11 +1510,11 @@
       <c r="C55" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>27</v>
@@ -1528,14 +1534,14 @@
       <c r="C56" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>17</v>
+      <c r="D56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>11</v>
@@ -1555,10 +1561,10 @@
         <v>19</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>27</v>
@@ -1584,7 +1590,7 @@
         <v>23</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4" t="s">
@@ -1625,7 +1631,7 @@
         <v>20</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>20</v>
@@ -1643,7 +1649,7 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
@@ -1660,8 +1666,12 @@
         <v>40</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
+      <c r="D62" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -1673,12 +1683,14 @@
       <c r="B63" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="4"/>
+      <c r="C63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="E63" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -1689,12 +1701,12 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="B64" s="4"/>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>

</xml_diff>

<commit_message>
el lunes adelanté la práctica del laboratorio todo el día, el martes seguí el horario, el miercoles traté de seguir el horario pero me estaba quedando dormido por lo que me dormí varias horas, el jueves tuve que apurarme a terminar la práctica del laboratorio porque es para hoy viernes 10 de marzo y hoy he seguido el horario. Fin
</commit_message>
<xml_diff>
--- a/horario informatica.xlsx
+++ b/horario informatica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="44">
   <si>
     <t>Semana del 13 al 19</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>parcial cálculo integral</t>
+  </si>
+  <si>
+    <t>estudiar algebrea lineal</t>
   </si>
 </sst>
 </file>
@@ -524,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,8 +1830,8 @@
       <c r="A75" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>9</v>
+      <c r="B75" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>16</v>
@@ -1847,13 +1850,15 @@
       <c r="A76" s="2">
         <v>0.5</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>9</v>
+      <c r="B76" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="6" t="s">
+      <c r="E76" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1861,10 +1866,14 @@
       <c r="A77" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B77" s="4"/>
+      <c r="B77" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
+      <c r="E77" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -1872,16 +1881,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="B78" s="4"/>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="1" t="s">
+      <c r="D78" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1890,19 +1899,19 @@
         <v>0.625</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -1910,16 +1919,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>27</v>
@@ -1929,32 +1938,34 @@
       <c r="A81" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>12</v>
+      <c r="B81" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F81" s="4"/>
+      <c r="F81" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>0.75</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>12</v>
+      <c r="B82" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>23</v>
+      <c r="D82" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>20</v>
@@ -1967,12 +1978,14 @@
       <c r="A83" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B83" s="4"/>
+      <c r="B83" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="C83" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>24</v>
+      <c r="D83" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>20</v>
@@ -2011,15 +2024,15 @@
       <c r="A86" s="2">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F86" s="4"/>
     </row>
@@ -2029,11 +2042,11 @@
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F87" s="4"/>
     </row>
@@ -2044,7 +2057,9 @@
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
+      <c r="E88" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F88" s="4"/>
     </row>
   </sheetData>

</xml_diff>